<commit_message>
Updating blueprint with tech mapping
</commit_message>
<xml_diff>
--- a/blueprint/Motivus_Enterprise_Migration_Blueprint_v1.0.xlsx
+++ b/blueprint/Motivus_Enterprise_Migration_Blueprint_v1.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/42c6230957050c53/Documents/Oracle/Oracle_Startups/Architecture_Engagements/Motivus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="8_{B91D35A7-CC39-B442-A94A-8A2A8702FE13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{66D2D9F0-01EC-D848-91BE-F81C9CF92F83}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="8_{B91D35A7-CC39-B442-A94A-8A2A8702FE13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B6B6A405-E027-8641-A929-D5D922C462FD}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-21100" windowWidth="38400" windowHeight="21100" tabRatio="830" activeTab="5" xr2:uid="{EE0B52EF-1061-4345-85A0-C1E6899EE87B}"/>
+    <workbookView xWindow="0" yWindow="-21600" windowWidth="38400" windowHeight="21600" tabRatio="830" activeTab="3" xr2:uid="{EE0B52EF-1061-4345-85A0-C1E6899EE87B}"/>
   </bookViews>
   <sheets>
     <sheet name="Start" sheetId="1" r:id="rId1"/>
@@ -19,14 +19,12 @@
     <sheet name="Network Input" sheetId="37" r:id="rId4"/>
     <sheet name="Compartment Input" sheetId="5" r:id="rId5"/>
     <sheet name="Network Design" sheetId="42" r:id="rId6"/>
-    <sheet name="Network Diagram" sheetId="10" r:id="rId7"/>
-    <sheet name="Compartment Design" sheetId="41" r:id="rId8"/>
-    <sheet name="Compartment Diagram" sheetId="11" r:id="rId9"/>
-    <sheet name="Brick Versions" sheetId="38" r:id="rId10"/>
-    <sheet name="Provider" sheetId="39" r:id="rId11"/>
-    <sheet name="Backend" sheetId="40" r:id="rId12"/>
-    <sheet name="Unit_Cost" sheetId="36" r:id="rId13"/>
-    <sheet name="CIDR Cheat Sheet" sheetId="44" state="hidden" r:id="rId14"/>
+    <sheet name="Compartment Design" sheetId="41" r:id="rId7"/>
+    <sheet name="Brick Versions" sheetId="38" r:id="rId8"/>
+    <sheet name="Provider" sheetId="39" r:id="rId9"/>
+    <sheet name="Backend" sheetId="40" r:id="rId10"/>
+    <sheet name="Unit_Cost" sheetId="36" r:id="rId11"/>
+    <sheet name="CIDR Cheat Sheet" sheetId="44" state="hidden" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Compartment Input'!$A$1:$B$8</definedName>
@@ -542,7 +540,7 @@
     <t>axyvvilklpqv</t>
   </si>
   <si>
-    <t>/home/ubuntu/REPOS/OCIFE/oci_infra/blueprint/network_design.png</t>
+    <t>PRD</t>
   </si>
 </sst>
 </file>
@@ -1359,6 +1357,159 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>365760</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>156978</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0D69502-E0C2-6B04-107D-6B0866906378}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7772400" cy="9097778"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFA9BC00-A9E9-68CB-3D7E-A6ED0A9B7ABF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12712700" cy="11087100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6BBA87F6-0124-1B94-CA66-5276AA987997}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="127000" y="101600"/>
+          <a:ext cx="8001000" cy="7251700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1659,7 +1810,7 @@
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="109" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1965,347 +2116,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3483BFDB-27F1-4B3B-BF2B-7D366733AD0D}">
-  <dimension ref="A1:D26"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="40.6640625" style="57" customWidth="1"/>
-    <col min="2" max="2" width="28.6640625" style="57" customWidth="1"/>
-    <col min="3" max="3" width="9" style="57"/>
-    <col min="4" max="4" width="79.33203125" style="57" customWidth="1"/>
-    <col min="5" max="16384" width="9" style="57"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="60" t="s">
-        <v>67</v>
-      </c>
-      <c r="B1" s="60" t="s">
-        <v>117</v>
-      </c>
-      <c r="C1" s="60" t="s">
-        <v>116</v>
-      </c>
-      <c r="D1" s="59" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="58" t="s">
-        <v>114</v>
-      </c>
-      <c r="B2" s="58" t="s">
-        <v>111</v>
-      </c>
-      <c r="C2" s="58" t="s">
-        <v>113</v>
-      </c>
-      <c r="D2" s="58" t="str">
-        <f t="shared" ref="D2:D26" si="0">IF(A2&lt;&gt;"",_xlfn.CONCAT("git::ssh://git@",B2,A2,".git?ref=",C2),"")</f>
-        <v>git::ssh://git@github.com/oracle-devrel/terraform-oci-cloudbricks-network-artifacts.git?ref=v2.0.1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="58" t="s">
-        <v>112</v>
-      </c>
-      <c r="B3" s="58" t="s">
-        <v>111</v>
-      </c>
-      <c r="C3" s="58" t="s">
-        <v>110</v>
-      </c>
-      <c r="D3" s="58" t="str">
-        <f t="shared" si="0"/>
-        <v>git::ssh://git@github.com/oracle-devrel/terraform-oci-cloudbricks-compartment.git?ref=v1.0.3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="69"/>
-      <c r="B4" s="58"/>
-      <c r="C4" s="69"/>
-      <c r="D4" s="58" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="58"/>
-      <c r="B5" s="58"/>
-      <c r="C5" s="58"/>
-      <c r="D5" s="58" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="58"/>
-      <c r="B6" s="58"/>
-      <c r="C6" s="58"/>
-      <c r="D6" s="58" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="58"/>
-      <c r="B7" s="58"/>
-      <c r="C7" s="58"/>
-      <c r="D7" s="58" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="58"/>
-      <c r="B8" s="58"/>
-      <c r="C8" s="58"/>
-      <c r="D8" s="58" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="58"/>
-      <c r="B9" s="58"/>
-      <c r="C9" s="58"/>
-      <c r="D9" s="58" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="58"/>
-      <c r="B10" s="58"/>
-      <c r="C10" s="58"/>
-      <c r="D10" s="58" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="58"/>
-      <c r="B11" s="58"/>
-      <c r="C11" s="58"/>
-      <c r="D11" s="58" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="58"/>
-      <c r="B12" s="58"/>
-      <c r="C12" s="58"/>
-      <c r="D12" s="58" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="58"/>
-      <c r="B13" s="58"/>
-      <c r="C13" s="58"/>
-      <c r="D13" s="58" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="58"/>
-      <c r="B14" s="58"/>
-      <c r="C14" s="58"/>
-      <c r="D14" s="58" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="58"/>
-      <c r="B15" s="58"/>
-      <c r="C15" s="58"/>
-      <c r="D15" s="58" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="58"/>
-      <c r="B16" s="58"/>
-      <c r="C16" s="58"/>
-      <c r="D16" s="58" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="58"/>
-      <c r="B17" s="58"/>
-      <c r="C17" s="58"/>
-      <c r="D17" s="58" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="58"/>
-      <c r="B18" s="58"/>
-      <c r="C18" s="58"/>
-      <c r="D18" s="58" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="58"/>
-      <c r="B19" s="58"/>
-      <c r="C19" s="58"/>
-      <c r="D19" s="58" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="58"/>
-      <c r="B20" s="58"/>
-      <c r="C20" s="58"/>
-      <c r="D20" s="58" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="58"/>
-      <c r="B21" s="58"/>
-      <c r="C21" s="58"/>
-      <c r="D21" s="58" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="58"/>
-      <c r="B22" s="58"/>
-      <c r="C22" s="58"/>
-      <c r="D22" s="58" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="58"/>
-      <c r="B23" s="58"/>
-      <c r="C23" s="58"/>
-      <c r="D23" s="58" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="58"/>
-      <c r="B24" s="58"/>
-      <c r="C24" s="58"/>
-      <c r="D24" s="58" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="58"/>
-      <c r="B25" s="58"/>
-      <c r="C25" s="58"/>
-      <c r="D25" s="58" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="58"/>
-      <c r="B26" s="58"/>
-      <c r="C26" s="58"/>
-      <c r="D26" s="58" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EA5D5F9-BE3E-47E0-87D3-59D4152AB4FB}">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16" style="57" customWidth="1"/>
-    <col min="2" max="2" width="70.33203125" style="57" customWidth="1"/>
-    <col min="3" max="16384" width="9" style="57"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="60" t="s">
-        <v>124</v>
-      </c>
-      <c r="B1" s="60" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="58" t="s">
-        <v>122</v>
-      </c>
-      <c r="B2" s="69" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="58" t="s">
-        <v>121</v>
-      </c>
-      <c r="B3" s="69" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="58" t="s">
-        <v>120</v>
-      </c>
-      <c r="B4" s="69" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="58" t="s">
-        <v>119</v>
-      </c>
-      <c r="B5" s="69" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="58" t="s">
-        <v>118</v>
-      </c>
-      <c r="B6" s="69" t="s">
-        <v>145</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BE7CBF6-B4FA-4FE1-8E37-775850BC4E41}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -2358,7 +2168,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D662B4F3-71A1-9244-8D27-D04D146F64BE}">
   <dimension ref="A1:G39"/>
   <sheetViews>
@@ -3033,7 +2843,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3552B68D-3FE7-4BED-84F7-316E0026221F}">
   <dimension ref="A1:G16"/>
   <sheetViews>
@@ -3193,13 +3003,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DABA704D-446B-5D46-8F38-BF168CC47E10}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="125" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4:R8"/>
+    <sheetView showGridLines="0" topLeftCell="A5" zoomScale="125" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3242,7 +3053,9 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="79"/>
+      <c r="A2" s="79" t="s">
+        <v>155</v>
+      </c>
       <c r="B2" s="24" t="s">
         <v>96</v>
       </c>
@@ -3298,8 +3111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A89CB4C-259D-43E2-9153-AB13BE28E364}">
   <dimension ref="A1:M148"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6222,7 +6035,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="A2" sqref="A2:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6390,17 +6203,300 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2629E1C-71BE-4876-A6E9-95DBA6ACA7A0}">
-  <dimension ref="O21"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4551179D-347F-47FD-B067-8D1D5A23E68E}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="N22" sqref="N22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3483BFDB-27F1-4B3B-BF2B-7D366733AD0D}">
+  <dimension ref="A1:D26"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="40.6640625" style="57" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" style="57" customWidth="1"/>
+    <col min="3" max="3" width="9" style="57"/>
+    <col min="4" max="4" width="79.33203125" style="57" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="57"/>
+  </cols>
   <sheetData>
-    <row r="21" spans="15:15" x14ac:dyDescent="0.2">
-      <c r="O21" t="s">
-        <v>155</v>
+    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="60" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="60" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1" s="60" t="s">
+        <v>116</v>
+      </c>
+      <c r="D1" s="59" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="58" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" s="58" t="s">
+        <v>111</v>
+      </c>
+      <c r="C2" s="58" t="s">
+        <v>113</v>
+      </c>
+      <c r="D2" s="58" t="str">
+        <f t="shared" ref="D2:D26" si="0">IF(A2&lt;&gt;"",_xlfn.CONCAT("git::ssh://git@",B2,A2,".git?ref=",C2),"")</f>
+        <v>git::ssh://git@github.com/oracle-devrel/terraform-oci-cloudbricks-network-artifacts.git?ref=v2.0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="58" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="58" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" s="58" t="s">
+        <v>110</v>
+      </c>
+      <c r="D3" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v>git::ssh://git@github.com/oracle-devrel/terraform-oci-cloudbricks-compartment.git?ref=v1.0.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="69"/>
+      <c r="B4" s="58"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="58"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="58"/>
+      <c r="B6" s="58"/>
+      <c r="C6" s="58"/>
+      <c r="D6" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="58"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="58"/>
+      <c r="B8" s="58"/>
+      <c r="C8" s="58"/>
+      <c r="D8" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="58"/>
+      <c r="B9" s="58"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="58"/>
+      <c r="B10" s="58"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="58"/>
+      <c r="B11" s="58"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="58"/>
+      <c r="B12" s="58"/>
+      <c r="C12" s="58"/>
+      <c r="D12" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="58"/>
+      <c r="B13" s="58"/>
+      <c r="C13" s="58"/>
+      <c r="D13" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="58"/>
+      <c r="B14" s="58"/>
+      <c r="C14" s="58"/>
+      <c r="D14" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="58"/>
+      <c r="B15" s="58"/>
+      <c r="C15" s="58"/>
+      <c r="D15" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="58"/>
+      <c r="B16" s="58"/>
+      <c r="C16" s="58"/>
+      <c r="D16" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="58"/>
+      <c r="B17" s="58"/>
+      <c r="C17" s="58"/>
+      <c r="D17" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="58"/>
+      <c r="B18" s="58"/>
+      <c r="C18" s="58"/>
+      <c r="D18" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="58"/>
+      <c r="B19" s="58"/>
+      <c r="C19" s="58"/>
+      <c r="D19" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="58"/>
+      <c r="B20" s="58"/>
+      <c r="C20" s="58"/>
+      <c r="D20" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="58"/>
+      <c r="B21" s="58"/>
+      <c r="C21" s="58"/>
+      <c r="D21" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="58"/>
+      <c r="B22" s="58"/>
+      <c r="C22" s="58"/>
+      <c r="D22" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="58"/>
+      <c r="B23" s="58"/>
+      <c r="C23" s="58"/>
+      <c r="D23" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="58"/>
+      <c r="B24" s="58"/>
+      <c r="C24" s="58"/>
+      <c r="D24" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="58"/>
+      <c r="B25" s="58"/>
+      <c r="C25" s="58"/>
+      <c r="D25" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="58"/>
+      <c r="B26" s="58"/>
+      <c r="C26" s="58"/>
+      <c r="D26" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -6408,44 +6504,70 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D7AC158-723D-5D4A-82EC-0FAFC572E38B}">
-  <dimension ref="A1"/>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EA5D5F9-BE3E-47E0-87D3-59D4152AB4FB}">
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="S1" zoomScale="87" zoomScaleNormal="163" workbookViewId="0">
-      <selection activeCell="AB26" sqref="AB26"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4551179D-347F-47FD-B067-8D1D5A23E68E}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="N28" sqref="N28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60BDE034-7FFF-D14F-8904-22D4A6F3769C}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16" style="57" customWidth="1"/>
+    <col min="2" max="2" width="70.33203125" style="57" customWidth="1"/>
+    <col min="3" max="16384" width="9" style="57"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="60" t="s">
+        <v>124</v>
+      </c>
+      <c r="B1" s="60" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="58" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" s="69" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="58" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" s="69" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="58" t="s">
+        <v>120</v>
+      </c>
+      <c r="B4" s="69" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="58" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5" s="69" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="58" t="s">
+        <v>118</v>
+      </c>
+      <c r="B6" s="69" t="s">
+        <v>145</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>